<commit_message>
1st draft of paper finished
</commit_message>
<xml_diff>
--- a/Python/Results Array.xlsx
+++ b/Python/Results Array.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\Lottery\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\KerkP\GIT Repositories\Lottery\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086C4154-3E47-42F0-9AE3-BADABB7D08B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328B0575-A291-488A-9A1E-5478E16B564B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="690" windowWidth="19440" windowHeight="19140" activeTab="4" xr2:uid="{B3EB2355-D439-41FF-A0B0-1141EA110A80}"/>
+    <workbookView xWindow="29190" yWindow="390" windowWidth="24375" windowHeight="15390" activeTab="2" xr2:uid="{B3EB2355-D439-41FF-A0B0-1141EA110A80}"/>
   </bookViews>
   <sheets>
     <sheet name="PDFs" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="68">
   <si>
     <t>list</t>
   </si>
@@ -204,16 +204,61 @@
   <si>
     <t>ratio2</t>
   </si>
+  <si>
+    <t>cdiff</t>
+  </si>
+  <si>
+    <t>udiff</t>
+  </si>
+  <si>
+    <t>Eulotterylose</t>
+  </si>
+  <si>
+    <t>Eulotterywin</t>
+  </si>
+  <si>
+    <t>2*Margu</t>
+  </si>
+  <si>
+    <t>cdiff/Ec</t>
+  </si>
+  <si>
+    <t>udiff/Eu</t>
+  </si>
+  <si>
+    <t>2*Margu/Eu</t>
+  </si>
+  <si>
+    <t>win/lose</t>
+  </si>
+  <si>
+    <t>Payoff</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>1.5 billion</t>
+  </si>
+  <si>
+    <t>226 million</t>
+  </si>
+  <si>
+    <t>23.3 trillion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="175" formatCode="0.000000000%"/>
+    <numFmt numFmtId="179" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="180" formatCode="0.0000000000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -356,7 +401,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -421,6 +466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -430,7 +476,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3289,7 +3384,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{A6BCAC31-CF9F-4CDB-A1CC-F9C19E6D05A4}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3301,7 +3396,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8669130" cy="6294783"/>
+    <xdr:ext cx="8664408" cy="6291513"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5073,59 +5168,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FA21F9-1524-4939-A076-9F03C746FDA3}">
-  <dimension ref="A1:O74"/>
+  <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="20" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="20" customWidth="1"/>
-    <col min="3" max="8" width="10.140625" customWidth="1"/>
+    <col min="3" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="8" width="10.140625" customWidth="1"/>
     <col min="11" max="14" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="71"/>
+      <c r="E1" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38" t="s">
+      <c r="F1" s="71"/>
+      <c r="G1" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="71"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="15" t="s">
+      <c r="A2" s="72"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="73" t="s">
         <v>18</v>
       </c>
       <c r="K2" s="8" t="s">
@@ -5136,28 +5234,28 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="55">
         <v>3</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="66">
         <v>-6.1932300240337297E-10</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="18">
         <v>2.99999999997089</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="10">
         <v>-6.1924110283939595E-10</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="7">
         <v>4.16636576383514E-5</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="7">
         <v>-6.1925110798659998E-10</v>
       </c>
       <c r="K3" t="s">
@@ -5168,28 +5266,28 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="55">
         <v>3</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="66">
         <v>-8.4307103929152802E-10</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="18">
         <v>2.9999999999854401</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="10">
         <v>-8.4296181146470396E-10</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="7">
         <v>4.3053275953585099E-5</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="7">
         <v>-8.4297706387517103E-10</v>
       </c>
       <c r="I4" s="11"/>
@@ -5202,56 +5300,56 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="55">
         <v>3</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="66">
         <v>-6.8587300066388601E-10</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="18">
         <v>3</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="10">
         <v>-6.8578132061958203E-10</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="7">
         <v>3.5294117231833898E-5</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="7">
         <v>-6.8579203883350499E-10</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="55">
         <v>3</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="66">
         <v>-1.08772484489558E-9</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="18">
         <v>2.99999999997089</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="10">
         <v>-1.0875790268372E-9</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="7">
         <v>4.16636576383514E-5</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="7">
         <v>-1.0876010243372899E-9</v>
       </c>
       <c r="K6" s="8" t="s">
@@ -5268,28 +5366,28 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="55">
         <v>3</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="66">
         <v>-1.8408499500647901E-9</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="18">
         <v>2.9999999999854401</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="10">
         <v>-1.84056658802944E-9</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="7">
         <v>4.3053275953585099E-5</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="7">
         <v>-1.84061117000361E-9</v>
       </c>
       <c r="K7" t="s">
@@ -5306,28 +5404,28 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="55">
         <v>3</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="66">
         <v>-1.5185619091508199E-9</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="18">
         <v>3</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="10">
         <v>-1.5183204693514E-9</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="7">
         <v>3.5294117231833898E-5</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="7">
         <v>-1.51835180890607E-9</v>
       </c>
       <c r="L8" t="s">
@@ -5338,28 +5436,28 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="55">
         <v>3</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="66">
         <v>-2.4645703651258601E-15</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="18">
         <v>2.99999999997089</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="10">
         <v>-2.46210333757842E-15</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="7">
         <v>4.16636576383514E-5</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="7">
         <v>2.00199799399541E-3</v>
       </c>
       <c r="I9" s="11"/>
@@ -5369,56 +5467,56 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="55">
         <v>3</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="66">
         <v>-6.0671101163679E-14</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="18">
         <v>2.9999999999854401</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="10">
         <v>-6.06103695732221E-14</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="7">
         <v>4.3053275953585099E-5</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="7">
         <v>2.0019979939932299E-3</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="55">
         <v>3</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="66">
         <v>-5.6217705904922901E-14</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="18">
         <v>3</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="10">
         <v>-5.61614321497752E-14</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="7">
         <v>3.5294117231833898E-5</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="7">
         <v>2.0019979939932399E-3</v>
       </c>
       <c r="K11" s="9" t="s">
@@ -5427,28 +5525,28 @@
       <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="55">
         <v>3</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="66">
         <v>-5.4537254328670404E-3</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="18">
         <v>2.99999999997089</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="10">
         <v>-5.36363156953711E-3</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="7">
         <v>4.16636576383514E-5</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="7">
         <v>-1.43256233412321E-5</v>
       </c>
       <c r="K12" s="9" t="s">
@@ -5457,28 +5555,28 @@
       <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="55">
         <v>3</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="66">
         <v>-5.7083408466750999E-3</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="18">
         <v>2.9999999999854401</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="10">
         <v>-5.6182059838079104E-3</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="7">
         <v>4.3053275953585099E-5</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="7">
         <v>-1.5383494175388902E-5</v>
       </c>
       <c r="K13" s="9" t="s">
@@ -5487,56 +5585,56 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="55">
         <v>3</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="66">
         <v>-5.2486619483199303E-3</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="18">
         <v>3</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="10">
         <v>-5.1586579140803198E-3</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="7">
         <v>3.5294117231833898E-5</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="7">
         <v>-1.2836313842713399E-5</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="55">
         <v>3</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="66">
         <v>-3.2311605115447099E-5</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="18">
         <v>2.99999999997089</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="10">
         <v>-3.2280933940142998E-5</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="7">
         <v>4.16636576383514E-5</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="7">
         <v>-2.9047209650894501E-6</v>
       </c>
       <c r="I15" s="11"/>
@@ -5546,28 +5644,28 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="55">
         <v>3</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="66">
         <v>-3.6185364516640701E-5</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="18">
         <v>2.9999999999854401</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="10">
         <v>-3.6154236441987503E-5</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="7">
         <v>4.3053275953585099E-5</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="7">
         <v>-3.27385780707878E-6</v>
       </c>
       <c r="K16" s="9" t="s">
@@ -5575,28 +5673,28 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="55">
         <v>3</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="66">
         <v>-3.1255951357502798E-5</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="18">
         <v>3</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="10">
         <v>-3.1225586653249498E-5</v>
       </c>
-      <c r="G17" s="30">
+      <c r="G17" s="7">
         <v>3.5294117231833898E-5</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="7">
         <v>-2.7817432984747901E-6</v>
       </c>
       <c r="K17" s="9" t="s">
@@ -5617,16 +5715,18 @@
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="A24" s="74"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="64" t="s">
         <v>46</v>
       </c>
       <c r="G24" t="s">
@@ -5636,22 +5736,24 @@
         <v>53</v>
       </c>
       <c r="I24" s="7"/>
-      <c r="L24" s="7" t="s">
+      <c r="K24" s="41"/>
+      <c r="L24" s="42" t="s">
         <v>47</v>
       </c>
+      <c r="M24" s="43"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="65">
         <f>Sheet4!F3</f>
         <v>-6.1924110283939595E-10</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="66">
         <f>F3</f>
         <v>-6.1924110283939595E-10</v>
       </c>
@@ -5659,662 +5761,1488 @@
         <f>Sheet2!F3</f>
         <v>-3.5441609647079899E-9</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="16">
         <f>Sheet3!F3</f>
         <v>-9.6483820932746702E-11</v>
       </c>
-      <c r="G25" s="39">
+      <c r="G25" s="36">
         <f>C25/D25</f>
         <v>1</v>
       </c>
       <c r="H25" s="18">
-        <f>E25/F25</f>
+        <f t="shared" ref="H25:H39" si="0">E25/F25</f>
         <v>36.733215273246898</v>
       </c>
       <c r="I25" s="7"/>
-      <c r="L25" s="9" t="s">
+      <c r="K25" s="44"/>
+      <c r="L25" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M25" s="9" t="s">
+      <c r="M25" s="33" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="65">
         <f>Sheet4!F4</f>
         <v>-8.4296181146470396E-10</v>
       </c>
-      <c r="D26" s="11">
-        <f t="shared" ref="D26:D39" si="0">F4</f>
+      <c r="D26" s="66">
+        <f t="shared" ref="D26:D39" si="1">F4</f>
         <v>-8.4296181146470396E-10</v>
       </c>
       <c r="E26" s="10">
         <f>Sheet2!F4</f>
         <v>-4.2986130210920204E-9</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="16">
         <f>Sheet3!F4</f>
         <v>-1.01718633516156E-10</v>
       </c>
-      <c r="G26" s="39">
-        <f t="shared" ref="G26:G39" si="1">C26/D26</f>
+      <c r="G26" s="36">
+        <f t="shared" ref="G26:G39" si="2">C26/D26</f>
         <v>1</v>
       </c>
       <c r="H26" s="18">
-        <f>E26/F26</f>
+        <f t="shared" si="0"/>
         <v>42.259838463217953</v>
       </c>
       <c r="I26" s="7"/>
-      <c r="K26" s="9" t="s">
+      <c r="K26" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="46">
         <v>0.10215829999999999</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="47">
         <v>0.100096</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="65">
         <f>Sheet4!F5</f>
         <v>-6.8578132061958203E-10</v>
       </c>
-      <c r="D27" s="11">
-        <f t="shared" si="0"/>
+      <c r="D27" s="66">
+        <f t="shared" si="1"/>
         <v>-6.8578132061958203E-10</v>
       </c>
       <c r="E27" s="10">
         <f>Sheet2!F5</f>
         <v>-3.3362553830684698E-9</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="16">
         <f>Sheet3!F5</f>
         <v>-9.52189438407913E-11</v>
       </c>
-      <c r="G27" s="39">
-        <f t="shared" si="1"/>
+      <c r="G27" s="36">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H27" s="18">
-        <f>E27/F27</f>
+        <f t="shared" si="0"/>
         <v>35.037727247287904</v>
       </c>
       <c r="I27" s="7"/>
-      <c r="K27" s="9" t="s">
+      <c r="K27" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="46">
         <v>0.101315</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="47">
         <v>9.8958000000000004E-2</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="65">
         <f>Sheet4!F6</f>
         <v>-1.0875790268372E-9</v>
       </c>
-      <c r="D28" s="11">
-        <f t="shared" si="0"/>
+      <c r="D28" s="66">
+        <f t="shared" si="1"/>
         <v>-1.0875790268372E-9</v>
       </c>
       <c r="E28" s="10">
         <f>Sheet2!F6</f>
         <v>-1.08430726619701E-8</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="16">
         <f>Sheet3!F6</f>
         <v>-1.1143386213774401E-10</v>
       </c>
-      <c r="G28" s="39">
-        <f t="shared" si="1"/>
+      <c r="G28" s="36">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H28" s="18">
-        <f>E28/F28</f>
+        <f t="shared" si="0"/>
         <v>97.305006341491762</v>
       </c>
       <c r="I28" s="7"/>
-      <c r="K28" s="9" t="s">
+      <c r="K28" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="48">
         <v>0.10329099999999999</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="49">
         <v>0.101149</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="65">
         <f>Sheet4!F7</f>
         <v>-1.84056658802944E-9</v>
       </c>
-      <c r="D29" s="11">
-        <f t="shared" si="0"/>
+      <c r="D29" s="66">
+        <f t="shared" si="1"/>
         <v>-1.84056658802944E-9</v>
       </c>
       <c r="E29" s="10">
         <f>Sheet2!F7</f>
         <v>-1.5207273662554101E-8</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F29" s="16">
         <f>Sheet3!F7</f>
         <v>-1.1794498711026299E-10</v>
       </c>
-      <c r="G29" s="39">
-        <f t="shared" si="1"/>
+      <c r="G29" s="36">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H29" s="18">
-        <f>E29/F29</f>
+        <f t="shared" si="0"/>
         <v>128.93531158163853</v>
       </c>
       <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="65">
         <f>Sheet4!F8</f>
         <v>-1.5183204693514E-9</v>
       </c>
-      <c r="D30" s="11">
-        <f t="shared" si="0"/>
+      <c r="D30" s="66">
+        <f t="shared" si="1"/>
         <v>-1.5183204693514E-9</v>
       </c>
       <c r="E30" s="10">
         <f>Sheet2!F8</f>
         <v>-1.0026316332734E-8</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F30" s="16">
         <f>Sheet3!F8</f>
         <v>-1.09870224029862E-10</v>
       </c>
-      <c r="G30" s="39">
-        <f t="shared" si="1"/>
+      <c r="G30" s="36">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H30" s="18">
-        <f>E30/F30</f>
+        <f t="shared" si="0"/>
         <v>91.255992433481467</v>
       </c>
       <c r="I30" s="7"/>
-      <c r="L30" s="7" t="s">
+      <c r="K30" s="41"/>
+      <c r="L30" s="42" t="s">
         <v>48</v>
       </c>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="43"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="65">
         <f>Sheet4!F9</f>
         <v>-2.46210333757842E-15</v>
       </c>
-      <c r="D31" s="11">
-        <f t="shared" si="0"/>
+      <c r="D31" s="66">
+        <f t="shared" si="1"/>
         <v>-2.46210333757842E-15</v>
       </c>
       <c r="E31" s="10">
         <f>Sheet2!F9</f>
         <v>-3.2642736485631298E-13</v>
       </c>
-      <c r="F31" s="10">
+      <c r="F31" s="16">
         <f>Sheet3!F9</f>
         <v>-2.5029301553482099E-65</v>
       </c>
-      <c r="G31" s="39">
-        <f t="shared" si="1"/>
+      <c r="G31" s="36">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H31" s="18">
-        <f>E31/F31</f>
+        <f t="shared" si="0"/>
         <v>1.3041808783949073E+52</v>
       </c>
       <c r="I31" s="18">
         <f>H31-H33</f>
         <v>5.2584259513251272E+39</v>
       </c>
-      <c r="L31" s="9" t="s">
+      <c r="K31" s="44"/>
+      <c r="L31" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="N31" s="9" t="s">
+      <c r="M31" s="46"/>
+      <c r="N31" s="45" t="s">
         <v>9</v>
       </c>
+      <c r="O31" s="47"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="65">
         <f>Sheet4!F10</f>
         <v>-6.06103695732221E-14</v>
       </c>
-      <c r="D32" s="11">
-        <f t="shared" si="0"/>
+      <c r="D32" s="66">
+        <f t="shared" si="1"/>
         <v>-6.06103695732221E-14</v>
       </c>
       <c r="E32" s="10">
         <f>Sheet2!F10</f>
         <v>-1.44830094012261E-12</v>
       </c>
-      <c r="F32" s="10">
+      <c r="F32" s="16">
         <f>Sheet3!F10</f>
         <v>-2.64273438607206E-64</v>
       </c>
-      <c r="G32" s="39">
-        <f t="shared" si="1"/>
+      <c r="G32" s="36">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H32" s="18">
-        <f>E32/F32</f>
+        <f t="shared" si="0"/>
         <v>5.4803121636270219E+51</v>
       </c>
       <c r="I32" s="7"/>
-      <c r="K32" s="9" t="s">
+      <c r="K32" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="46">
         <v>26000</v>
       </c>
-      <c r="M32" s="19">
+      <c r="M32" s="51">
         <f>150000000/(L32*2)</f>
         <v>2884.6153846153848</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="46">
         <v>18600</v>
       </c>
-      <c r="O32" s="19">
+      <c r="O32" s="52">
         <f>150000000/(N32*2)</f>
         <v>4032.2580645161293</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="65">
         <f>Sheet4!F11</f>
         <v>-5.61614321497752E-14</v>
       </c>
-      <c r="D33" s="11">
-        <f t="shared" si="0"/>
+      <c r="D33" s="66">
+        <f t="shared" si="1"/>
         <v>-5.61614321497752E-14</v>
       </c>
       <c r="E33" s="10">
         <f>Sheet2!F11</f>
         <v>-4.2930716224039998E-13</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F33" s="16">
         <f>Sheet3!F11</f>
         <v>-3.2917762355857701E-65</v>
       </c>
-      <c r="G33" s="39">
-        <f t="shared" si="1"/>
+      <c r="G33" s="36">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H33" s="18">
-        <f>E33/F33</f>
+        <f t="shared" si="0"/>
         <v>1.3041808783943814E+52</v>
       </c>
       <c r="I33" s="7"/>
-      <c r="K33" s="9" t="s">
+      <c r="K33" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="46">
         <v>21500</v>
       </c>
-      <c r="M33" s="19">
+      <c r="M33" s="51">
         <f>150000000/(L33*2)</f>
         <v>3488.3720930232557</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="46">
         <v>13200</v>
       </c>
-      <c r="O33" s="19">
+      <c r="O33" s="52">
         <f>150000000/(N33*2)</f>
         <v>5681.818181818182</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="65">
         <f>Sheet4!F12</f>
         <v>-5.4753311624722301E-3</v>
       </c>
-      <c r="D34" s="11">
-        <f t="shared" si="0"/>
+      <c r="D34" s="66">
+        <f t="shared" si="1"/>
         <v>-5.36363156953711E-3</v>
       </c>
       <c r="E34" s="10">
         <f>Sheet2!F12</f>
         <v>-8.8757331977546896E-3</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F34" s="16">
         <f>Sheet3!F12</f>
         <v>-3.5398096985090801E-3</v>
       </c>
-      <c r="G34" s="39">
-        <f t="shared" si="1"/>
+      <c r="G34" s="36">
+        <f t="shared" si="2"/>
         <v>1.0208253664493887</v>
       </c>
       <c r="H34" s="18">
-        <f>E34/F34</f>
+        <f t="shared" si="0"/>
         <v>2.5074040566341824</v>
       </c>
       <c r="I34" s="7"/>
-      <c r="K34" s="9" t="s">
+      <c r="K34" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="48">
         <v>22700</v>
       </c>
-      <c r="M34" s="19">
+      <c r="M34" s="53">
         <f>150000000/(L34*2)</f>
         <v>3303.964757709251</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="48">
         <v>13600</v>
       </c>
-      <c r="O34" s="19">
+      <c r="O34" s="54">
         <f>150000000/(N34*2)</f>
         <v>5514.7058823529414</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="65">
         <f>Sheet4!F13</f>
         <v>-5.7299057996829097E-3</v>
       </c>
-      <c r="D35" s="11">
-        <f t="shared" si="0"/>
+      <c r="D35" s="66">
+        <f t="shared" si="1"/>
         <v>-5.6182059838079104E-3</v>
       </c>
       <c r="E35" s="10">
         <f>Sheet2!F13</f>
         <v>-9.3230362363101397E-3</v>
       </c>
-      <c r="F35" s="10">
+      <c r="F35" s="16">
         <f>Sheet3!F13</f>
         <v>-3.5893406794684701E-3</v>
       </c>
-      <c r="G35" s="39">
-        <f t="shared" si="1"/>
+      <c r="G35" s="36">
+        <f t="shared" si="2"/>
         <v>1.0198817587316888</v>
       </c>
       <c r="H35" s="18">
-        <f>E35/F35</f>
+        <f t="shared" si="0"/>
         <v>2.5974230558941391</v>
       </c>
       <c r="I35" s="7"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="V35" s="46"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="65">
         <f>Sheet4!F14</f>
         <v>-5.2703562608940003E-3</v>
       </c>
-      <c r="D36" s="11">
-        <f t="shared" si="0"/>
+      <c r="D36" s="66">
+        <f t="shared" si="1"/>
         <v>-5.1586579140803198E-3</v>
       </c>
       <c r="E36" s="10">
         <f>Sheet2!F14</f>
         <v>-8.7186773878329404E-3</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F36" s="16">
         <f>Sheet3!F14</f>
         <v>-3.5273062479745901E-3</v>
       </c>
-      <c r="G36" s="39">
-        <f t="shared" si="1"/>
+      <c r="G36" s="36">
+        <f t="shared" si="2"/>
         <v>1.0216525981513147</v>
       </c>
       <c r="H36" s="18">
-        <f>E36/F36</f>
+        <f t="shared" si="0"/>
         <v>2.4717664911685171</v>
       </c>
       <c r="I36" s="7"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+      <c r="N36" t="s">
+        <v>54</v>
+      </c>
+      <c r="O36" t="s">
+        <v>55</v>
+      </c>
+      <c r="P36" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>57</v>
+      </c>
+      <c r="R36" t="s">
+        <v>58</v>
+      </c>
+      <c r="S36" t="s">
+        <v>59</v>
+      </c>
+      <c r="T36" t="s">
+        <v>60</v>
+      </c>
+      <c r="U36" t="s">
+        <v>61</v>
+      </c>
+      <c r="V36" s="46"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="65">
         <f>Sheet4!F15</f>
         <v>-3.2287241989337102E-5</v>
       </c>
-      <c r="D37" s="11">
-        <f t="shared" si="0"/>
+      <c r="D37" s="66">
+        <f t="shared" si="1"/>
         <v>-3.2280933940142998E-5</v>
       </c>
       <c r="E37" s="10">
         <f>Sheet2!F15</f>
         <v>-8.38724432838944E-5</v>
       </c>
-      <c r="F37" s="10">
+      <c r="F37" s="16">
         <f>Sheet3!F15</f>
         <v>-1.38607778552568E-5</v>
       </c>
-      <c r="G37" s="39">
-        <f t="shared" si="1"/>
+      <c r="G37" s="36">
+        <f t="shared" si="2"/>
         <v>1.0001954109879783</v>
       </c>
       <c r="H37" s="18">
-        <f>E37/F37</f>
+        <f t="shared" si="0"/>
         <v>6.0510632346715783</v>
       </c>
       <c r="I37" s="7"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+      <c r="K37" t="s">
+        <v>66</v>
+      </c>
+      <c r="L37" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" t="s">
+        <v>8</v>
+      </c>
+      <c r="N37">
+        <v>-1.2466666666878099</v>
+      </c>
+      <c r="O37" s="11">
+        <v>-6.1924110283939595E-10</v>
+      </c>
+      <c r="P37">
+        <v>0.99998383919752198</v>
+      </c>
+      <c r="Q37" s="11">
+        <v>3.33333331858876E-9</v>
+      </c>
+      <c r="R37" s="11">
+        <v>-6.1932298988551197E-10</v>
+      </c>
+      <c r="S37" s="11">
+        <v>-1.7313564396843201E-5</v>
+      </c>
+      <c r="T37" s="11">
+        <v>-6.1925110798659998E-10</v>
+      </c>
+      <c r="U37" s="11">
+        <v>-6.1933299635577402E-10</v>
+      </c>
+      <c r="V37" s="76"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="65">
         <f>Sheet4!F16</f>
         <v>-3.61605445213797E-5</v>
       </c>
-      <c r="D38" s="11">
-        <f t="shared" si="0"/>
+      <c r="D38" s="66">
+        <f t="shared" si="1"/>
         <v>-3.6154236441987503E-5</v>
       </c>
       <c r="E38" s="10">
         <f>Sheet2!F16</f>
         <v>-9.2497661977830603E-5</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38" s="16">
         <f>Sheet3!F16</f>
         <v>-1.42338449062862E-5</v>
       </c>
-      <c r="G38" s="39">
-        <f t="shared" si="1"/>
+      <c r="G38" s="36">
+        <f t="shared" si="2"/>
         <v>1.0001744769081853</v>
       </c>
       <c r="H38" s="18">
-        <f>E38/F38</f>
+        <f t="shared" si="0"/>
         <v>6.4984312100365917</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="K38" t="s">
+        <v>66</v>
+      </c>
+      <c r="L38" t="s">
+        <v>7</v>
+      </c>
+      <c r="M38" t="s">
+        <v>9</v>
+      </c>
+      <c r="N38">
+        <v>-1.2466666666878099</v>
+      </c>
+      <c r="O38" s="11">
+        <v>-1.0875790268372E-9</v>
+      </c>
+      <c r="P38">
+        <v>0.99997976987168302</v>
+      </c>
+      <c r="Q38" s="11">
+        <v>3.3333333185881098E-9</v>
+      </c>
+      <c r="R38" s="11">
+        <v>-1.08772483237645E-9</v>
+      </c>
+      <c r="S38" s="11">
+        <v>-1.7313564396843201E-5</v>
+      </c>
+      <c r="T38" s="11">
+        <v>-1.0876010243372899E-9</v>
+      </c>
+      <c r="U38" s="11">
+        <v>-1.0877468328256201E-9</v>
+      </c>
+      <c r="V38" s="76"/>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="67">
         <f>Sheet4!F17</f>
         <v>-3.1231894540795197E-5</v>
       </c>
-      <c r="D39" s="11">
-        <f t="shared" si="0"/>
+      <c r="D39" s="68">
+        <f t="shared" si="1"/>
         <v>-3.1225586653249498E-5</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39" s="69">
         <f>Sheet2!F17</f>
         <v>-8.1082068133397897E-5</v>
       </c>
-      <c r="F39" s="10">
+      <c r="F39" s="17">
         <f>Sheet3!F17</f>
         <v>-1.37679637575161E-5</v>
       </c>
-      <c r="G39" s="39">
-        <f t="shared" si="1"/>
+      <c r="G39" s="36">
+        <f t="shared" si="2"/>
         <v>1.0002020102173179</v>
       </c>
       <c r="H39" s="18">
-        <f>E39/F39</f>
+        <f t="shared" si="0"/>
         <v>5.8891837283588293</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
+        <v>66</v>
+      </c>
+      <c r="L39" t="s">
+        <v>7</v>
+      </c>
+      <c r="M39" t="s">
+        <v>10</v>
+      </c>
+      <c r="N39">
+        <v>-1.2466666666878099</v>
+      </c>
+      <c r="O39" s="11">
+        <v>-2.4424906541753401E-15</v>
+      </c>
+      <c r="P39">
+        <v>0.99999999666543404</v>
+      </c>
+      <c r="Q39" s="11">
+        <v>3.3333333333333301E-9</v>
+      </c>
+      <c r="R39" s="11">
+        <v>-2.4645703651258601E-15</v>
+      </c>
+      <c r="S39" s="11">
+        <v>-1.7313564396843201E-5</v>
+      </c>
+      <c r="T39" s="11">
+        <v>-2.4424906541783401E-15</v>
+      </c>
+      <c r="U39" s="11">
+        <v>-2.4645703651288999E-15</v>
+      </c>
+      <c r="V39" s="76"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>66</v>
+      </c>
+      <c r="L40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M40" t="s">
+        <v>11</v>
+      </c>
+      <c r="N40">
+        <v>-1.2466666666878099</v>
+      </c>
+      <c r="O40">
+        <v>-1.5488767712668001E-4</v>
+      </c>
+      <c r="P40">
+        <v>10007.197359129599</v>
+      </c>
+      <c r="Q40" s="11">
+        <v>7.83258156091887E-5</v>
+      </c>
+      <c r="R40">
+        <v>-1.6779635400943801E-4</v>
+      </c>
+      <c r="S40" s="11">
+        <v>-1.7313564396843201E-5</v>
+      </c>
+      <c r="T40" s="11">
+        <v>-1.5477627547315601E-8</v>
+      </c>
+      <c r="U40" s="11">
+        <v>-1.6767566789909799E-8</v>
+      </c>
+      <c r="V40" s="40"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H41">
         <f>MIN(H25:H38)</f>
         <v>2.4717664911685171</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>66</v>
+      </c>
+      <c r="L41" t="s">
+        <v>7</v>
+      </c>
+      <c r="M41" t="s">
+        <v>12</v>
+      </c>
+      <c r="N41">
+        <v>-1.2466666666878099</v>
+      </c>
+      <c r="O41" s="11">
+        <v>-3.2287241989337102E-5</v>
+      </c>
+      <c r="P41">
+        <v>11.113232684457101</v>
+      </c>
+      <c r="Q41" s="11">
+        <v>6.4121213660378796E-8</v>
+      </c>
+      <c r="R41" s="11">
+        <v>-3.2311606017060498E-5</v>
+      </c>
+      <c r="S41" s="11">
+        <v>-1.7313564396843201E-5</v>
+      </c>
+      <c r="T41" s="11">
+        <v>-2.9052885794830402E-6</v>
+      </c>
+      <c r="U41" s="11">
+        <v>-2.9074809169864498E-6</v>
+      </c>
+      <c r="V41" s="40"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H42">
         <f>MAX(H25:H38)</f>
         <v>1.3041808783949073E+52</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="20">
+      <c r="K42" t="s">
+        <v>65</v>
+      </c>
+      <c r="L42" t="s">
+        <v>7</v>
+      </c>
+      <c r="M42" t="s">
+        <v>8</v>
+      </c>
+      <c r="N42">
+        <v>2.99999999997089</v>
+      </c>
+      <c r="O42" s="11">
+        <v>-6.1924110283939595E-10</v>
+      </c>
+      <c r="P42">
+        <v>0.99998383919752198</v>
+      </c>
+      <c r="Q42" s="11">
+        <v>3.3333333311112099E-9</v>
+      </c>
+      <c r="R42" s="11">
+        <v>-6.1932300240337297E-10</v>
+      </c>
+      <c r="S42" s="11">
+        <v>4.16636576383514E-5</v>
+      </c>
+      <c r="T42" s="11">
+        <v>-6.1925110798659998E-10</v>
+      </c>
+      <c r="U42" s="11">
+        <v>-6.1933300887383696E-10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K43" t="s">
+        <v>65</v>
+      </c>
+      <c r="L43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M43" t="s">
+        <v>9</v>
+      </c>
+      <c r="N43">
+        <v>2.99999999997089</v>
+      </c>
+      <c r="O43" s="11">
+        <v>-1.0875790268372E-9</v>
+      </c>
+      <c r="P43">
+        <v>0.99997976987168302</v>
+      </c>
+      <c r="Q43" s="11">
+        <v>3.3333333311112E-9</v>
+      </c>
+      <c r="R43" s="11">
+        <v>-1.08772484489558E-9</v>
+      </c>
+      <c r="S43" s="11">
+        <v>4.16636576383514E-5</v>
+      </c>
+      <c r="T43" s="11">
+        <v>-1.0876010243372899E-9</v>
+      </c>
+      <c r="U43" s="11">
+        <v>-1.08774684534501E-9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A44" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="50" t="str">
+        <f>P36</f>
+        <v>Eulotterylose</v>
+      </c>
+      <c r="D44" s="50" t="str">
+        <f>Q36</f>
+        <v>Eulotterywin</v>
+      </c>
+      <c r="E44" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="K44" t="s">
+        <v>65</v>
+      </c>
+      <c r="L44" t="s">
+        <v>7</v>
+      </c>
+      <c r="M44" t="s">
+        <v>10</v>
+      </c>
+      <c r="N44">
+        <v>2.99999999997089</v>
+      </c>
+      <c r="O44" s="11">
+        <v>-2.4424906541753401E-15</v>
+      </c>
+      <c r="P44">
+        <v>0.99999999666543404</v>
+      </c>
+      <c r="Q44" s="11">
+        <v>3.3333333333333301E-9</v>
+      </c>
+      <c r="R44" s="11">
+        <v>-2.4645703651258601E-15</v>
+      </c>
+      <c r="S44" s="11">
+        <v>4.16636576383514E-5</v>
+      </c>
+      <c r="T44" s="11">
+        <v>-2.4424906541783401E-15</v>
+      </c>
+      <c r="U44" s="11">
+        <v>-2.4645703651288999E-15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45" s="44" t="str">
+        <f>K37</f>
+        <v>226 million</v>
+      </c>
+      <c r="B45" s="46" t="str">
+        <f>M37</f>
+        <v>CRRA</v>
+      </c>
+      <c r="C45" s="55">
+        <f>P37</f>
+        <v>0.99998383919752198</v>
+      </c>
+      <c r="D45" s="56">
+        <f>Q37</f>
+        <v>3.33333331858876E-9</v>
+      </c>
+      <c r="E45" s="57">
+        <f>D45/C45</f>
+        <v>3.3333871888007009E-9</v>
+      </c>
+      <c r="K45" t="s">
+        <v>65</v>
+      </c>
+      <c r="L45" t="s">
+        <v>7</v>
+      </c>
+      <c r="M45" t="s">
+        <v>11</v>
+      </c>
+      <c r="N45">
+        <v>2.99999999997089</v>
+      </c>
+      <c r="O45" s="11">
+        <v>-4.7617037125746699E-5</v>
+      </c>
+      <c r="P45">
+        <v>10007.197359129599</v>
+      </c>
+      <c r="Q45">
+        <v>1.85596456089907E-4</v>
+      </c>
+      <c r="R45">
+        <v>-1.1005560321605199E-4</v>
+      </c>
+      <c r="S45" s="11">
+        <v>4.16636576383514E-5</v>
+      </c>
+      <c r="T45" s="11">
+        <v>-4.7582788973988304E-9</v>
+      </c>
+      <c r="U45" s="11">
+        <v>-1.09976446653017E-8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A46" s="44" t="str">
+        <f t="shared" ref="A46:A61" si="3">K38</f>
+        <v>226 million</v>
+      </c>
+      <c r="B46" s="46" t="str">
+        <f t="shared" ref="B46:B61" si="4">M38</f>
+        <v>S-G</v>
+      </c>
+      <c r="C46" s="55">
+        <f t="shared" ref="C46:D46" si="5">P38</f>
+        <v>0.99997976987168302</v>
+      </c>
+      <c r="D46" s="56">
+        <f t="shared" si="5"/>
+        <v>3.3333333185881098E-9</v>
+      </c>
+      <c r="E46" s="57">
+        <f t="shared" ref="E46:E61" si="6">D46/C46</f>
+        <v>3.3334007537130892E-9</v>
+      </c>
+      <c r="K46" t="s">
+        <v>65</v>
+      </c>
+      <c r="L46" t="s">
+        <v>7</v>
+      </c>
+      <c r="M46" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="20">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="20">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="20" t="s">
-        <v>6</v>
-      </c>
+      <c r="N46">
+        <v>2.99999999997089</v>
+      </c>
+      <c r="O46" s="11">
+        <v>-3.2280933940142998E-5</v>
+      </c>
+      <c r="P46">
+        <v>11.113232684457101</v>
+      </c>
+      <c r="Q46" s="11">
+        <v>7.0429263152952196E-8</v>
+      </c>
+      <c r="R46" s="11">
+        <v>-3.2311605115447099E-5</v>
+      </c>
+      <c r="S46" s="11">
+        <v>4.16636576383514E-5</v>
+      </c>
+      <c r="T46" s="11">
+        <v>-2.9047209650894501E-6</v>
+      </c>
+      <c r="U46" s="11">
+        <v>-2.9074808358569701E-6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A47" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>226 million</v>
+      </c>
+      <c r="B47" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>exponential</v>
+      </c>
+      <c r="C47" s="55">
+        <f t="shared" ref="C47:D47" si="7">P39</f>
+        <v>0.99999999666543404</v>
+      </c>
+      <c r="D47" s="56">
+        <f t="shared" si="7"/>
+        <v>3.3333333333333301E-9</v>
+      </c>
+      <c r="E47" s="57">
+        <f t="shared" si="6"/>
+        <v>3.3333333444485501E-9</v>
+      </c>
+      <c r="K47" t="s">
+        <v>67</v>
+      </c>
+      <c r="L47" t="s">
+        <v>7</v>
+      </c>
+      <c r="M47" t="s">
+        <v>8</v>
+      </c>
+      <c r="N47">
+        <v>77331.333333333299</v>
+      </c>
+      <c r="O47" s="11">
+        <v>-6.1924099181709297E-10</v>
+      </c>
+      <c r="P47">
+        <v>0.99998383919752198</v>
+      </c>
+      <c r="Q47" s="11">
+        <v>3.3333333333331899E-9</v>
+      </c>
+      <c r="R47" s="11">
+        <v>-6.19323004625238E-10</v>
+      </c>
+      <c r="S47" s="11">
+        <v>1.07396873224949</v>
+      </c>
+      <c r="T47" s="11">
+        <v>-6.1925099696250399E-10</v>
+      </c>
+      <c r="U47" s="11">
+        <v>-6.1933301109573797E-10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A48" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>226 million</v>
+      </c>
+      <c r="B48" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>HARA</v>
+      </c>
+      <c r="C48" s="55">
+        <f t="shared" ref="C48:D48" si="8">P40</f>
+        <v>10007.197359129599</v>
+      </c>
+      <c r="D48" s="56">
+        <f t="shared" si="8"/>
+        <v>7.83258156091887E-5</v>
+      </c>
+      <c r="E48" s="57">
+        <f t="shared" si="6"/>
+        <v>7.8269482251923211E-9</v>
+      </c>
+      <c r="K48" t="s">
+        <v>67</v>
+      </c>
+      <c r="L48" t="s">
+        <v>7</v>
+      </c>
+      <c r="M48" t="s">
+        <v>9</v>
+      </c>
+      <c r="N48">
+        <v>77331.333333333299</v>
+      </c>
+      <c r="O48" s="11">
+        <v>-1.0875789158149E-9</v>
+      </c>
+      <c r="P48">
+        <v>0.99997976987168302</v>
+      </c>
+      <c r="Q48" s="11">
+        <v>3.3333333333331899E-9</v>
+      </c>
+      <c r="R48" s="11">
+        <v>-1.08772484711748E-9</v>
+      </c>
+      <c r="S48" s="11">
+        <v>1.07396873224949</v>
+      </c>
+      <c r="T48" s="11">
+        <v>-1.08760091331274E-9</v>
+      </c>
+      <c r="U48" s="11">
+        <v>-1.0877468475669501E-9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>226 million</v>
+      </c>
+      <c r="B49" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>log</v>
+      </c>
+      <c r="C49" s="55">
+        <f t="shared" ref="C49:D49" si="9">P41</f>
+        <v>11.113232684457101</v>
+      </c>
+      <c r="D49" s="56">
+        <f t="shared" si="9"/>
+        <v>6.4121213660378796E-8</v>
+      </c>
+      <c r="E49" s="57">
+        <f t="shared" si="6"/>
+        <v>5.7698075331454485E-9</v>
+      </c>
+      <c r="K49" t="s">
+        <v>67</v>
+      </c>
+      <c r="L49" t="s">
+        <v>7</v>
+      </c>
+      <c r="M49" t="s">
+        <v>10</v>
+      </c>
+      <c r="N49">
+        <v>77331.333333333299</v>
+      </c>
+      <c r="O49" s="11">
+        <v>-2.4424906541753401E-15</v>
+      </c>
+      <c r="P49">
+        <v>0.99999999666543404</v>
+      </c>
+      <c r="Q49" s="11">
+        <v>3.3333333333333301E-9</v>
+      </c>
+      <c r="R49" s="11">
+        <v>-2.4645703651258601E-15</v>
+      </c>
+      <c r="S49" s="11">
+        <v>1.07396873224949</v>
+      </c>
+      <c r="T49" s="11">
+        <v>-2.4424906541783401E-15</v>
+      </c>
+      <c r="U49" s="11">
+        <v>-2.4645703651288999E-15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>1.5 billion</v>
+      </c>
+      <c r="B50" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>CRRA</v>
+      </c>
+      <c r="C50" s="55">
+        <f t="shared" ref="C50:D50" si="10">P42</f>
+        <v>0.99998383919752198</v>
+      </c>
+      <c r="D50" s="56">
+        <f t="shared" si="10"/>
+        <v>3.3333333311112099E-9</v>
+      </c>
+      <c r="E50" s="57">
+        <f t="shared" si="6"/>
+        <v>3.3333872013233531E-9</v>
+      </c>
+      <c r="K50" t="s">
+        <v>67</v>
+      </c>
+      <c r="L50" t="s">
+        <v>7</v>
+      </c>
+      <c r="M50" t="s">
+        <v>11</v>
+      </c>
+      <c r="N50">
+        <v>77331.333333333299</v>
+      </c>
+      <c r="O50" s="11">
+        <v>2.24726594969979E-2</v>
+      </c>
+      <c r="P50">
+        <v>10007.197359129599</v>
+      </c>
+      <c r="Q50">
+        <v>2.2705872990632502E-2</v>
+      </c>
+      <c r="R50">
+        <v>1.11530558241189E-2</v>
+      </c>
+      <c r="S50" s="11">
+        <v>1.07396873224949</v>
+      </c>
+      <c r="T50" s="11">
+        <v>2.24564962264686E-6</v>
+      </c>
+      <c r="U50" s="11">
+        <v>1.1145034082920999E-6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>1.5 billion</v>
+      </c>
+      <c r="B51" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>S-G</v>
+      </c>
+      <c r="C51" s="55">
+        <f t="shared" ref="C51:D51" si="11">P43</f>
+        <v>0.99997976987168302</v>
+      </c>
+      <c r="D51" s="56">
+        <f t="shared" si="11"/>
+        <v>3.3333333311112E-9</v>
+      </c>
+      <c r="E51" s="57">
+        <f t="shared" si="6"/>
+        <v>3.3334007662364329E-9</v>
+      </c>
+      <c r="K51" t="s">
+        <v>67</v>
+      </c>
+      <c r="L51" t="s">
+        <v>7</v>
+      </c>
+      <c r="M51" t="s">
+        <v>12</v>
+      </c>
+      <c r="N51">
+        <v>77331.333333333299</v>
+      </c>
+      <c r="O51" s="11">
+        <v>-3.2248779291421602E-5</v>
+      </c>
+      <c r="P51">
+        <v>11.113232684457101</v>
+      </c>
+      <c r="Q51" s="11">
+        <v>1.02583911325681E-7</v>
+      </c>
+      <c r="R51" s="11">
+        <v>-3.2311604955459001E-5</v>
+      </c>
+      <c r="S51" s="11">
+        <v>1.07396873224949</v>
+      </c>
+      <c r="T51" s="11">
+        <v>-2.9018276075912E-6</v>
+      </c>
+      <c r="U51" s="11">
+        <v>-2.90748082146084E-6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>1.5 billion</v>
+      </c>
+      <c r="B52" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>exponential</v>
+      </c>
+      <c r="C52" s="55">
+        <f t="shared" ref="C52:D52" si="12">P44</f>
+        <v>0.99999999666543404</v>
+      </c>
+      <c r="D52" s="56">
+        <f t="shared" si="12"/>
+        <v>3.3333333333333301E-9</v>
+      </c>
+      <c r="E52" s="57">
+        <f t="shared" si="6"/>
+        <v>3.3333333444485501E-9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A53" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>1.5 billion</v>
+      </c>
+      <c r="B53" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>HARA</v>
+      </c>
+      <c r="C53" s="55">
+        <f t="shared" ref="C53:D53" si="13">P45</f>
+        <v>10007.197359129599</v>
+      </c>
+      <c r="D53" s="56">
+        <f t="shared" si="13"/>
+        <v>1.85596456089907E-4</v>
+      </c>
+      <c r="E53" s="57">
+        <f t="shared" si="6"/>
+        <v>1.8546297172862965E-8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A54" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>1.5 billion</v>
+      </c>
+      <c r="B54" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>log</v>
+      </c>
+      <c r="C54" s="55">
+        <f t="shared" ref="C54:D54" si="14">P46</f>
+        <v>11.113232684457101</v>
+      </c>
+      <c r="D54" s="56">
+        <f t="shared" si="14"/>
+        <v>7.0429263152952196E-8</v>
+      </c>
+      <c r="E54" s="57">
+        <f t="shared" si="6"/>
+        <v>6.3374236059552803E-9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A55" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>23.3 trillion</v>
+      </c>
+      <c r="B55" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>CRRA</v>
+      </c>
+      <c r="C55" s="55">
+        <f t="shared" ref="C55:D55" si="15">P47</f>
+        <v>0.99998383919752198</v>
+      </c>
+      <c r="D55" s="56">
+        <f t="shared" si="15"/>
+        <v>3.3333333333331899E-9</v>
+      </c>
+      <c r="E55" s="57">
+        <f t="shared" si="6"/>
+        <v>3.333387203545369E-9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A56" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>23.3 trillion</v>
+      </c>
+      <c r="B56" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>S-G</v>
+      </c>
+      <c r="C56" s="55">
+        <f t="shared" ref="C56:D56" si="16">P48</f>
+        <v>0.99997976987168302</v>
+      </c>
+      <c r="D56" s="56">
+        <f t="shared" si="16"/>
+        <v>3.3333333333331899E-9</v>
+      </c>
+      <c r="E56" s="57">
+        <f t="shared" si="6"/>
+        <v>3.3334007684584679E-9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A57" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>23.3 trillion</v>
+      </c>
+      <c r="B57" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>exponential</v>
+      </c>
+      <c r="C57" s="55">
+        <f t="shared" ref="C57:D57" si="17">P49</f>
+        <v>0.99999999666543404</v>
+      </c>
+      <c r="D57" s="56">
+        <f t="shared" si="17"/>
+        <v>3.3333333333333301E-9</v>
+      </c>
+      <c r="E57" s="57">
+        <f t="shared" si="6"/>
+        <v>3.3333333444485501E-9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v>23.3 trillion</v>
+      </c>
+      <c r="B58" s="46" t="str">
+        <f t="shared" si="4"/>
+        <v>HARA</v>
+      </c>
+      <c r="C58" s="55">
+        <f t="shared" ref="C58:D58" si="18">P50</f>
+        <v>10007.197359129599</v>
+      </c>
+      <c r="D58" s="56">
+        <f t="shared" si="18"/>
+        <v>2.2705872990632502E-2</v>
+      </c>
+      <c r="E58" s="57">
+        <f t="shared" si="6"/>
+        <v>2.2689542512037957E-6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A59" s="58" t="str">
+        <f t="shared" si="3"/>
+        <v>23.3 trillion</v>
+      </c>
+      <c r="B59" s="48" t="str">
+        <f t="shared" si="4"/>
+        <v>log</v>
+      </c>
+      <c r="C59" s="59">
+        <f t="shared" ref="C59:D59" si="19">P51</f>
+        <v>11.113232684457101</v>
+      </c>
+      <c r="D59" s="60">
+        <f t="shared" si="19"/>
+        <v>1.02583911325681E-7</v>
+      </c>
+      <c r="E59" s="61">
+        <f t="shared" si="6"/>
+        <v>9.2307894775886621E-9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A60" s="44"/>
+      <c r="B60" s="46"/>
+      <c r="C60" s="55"/>
+      <c r="D60" s="56"/>
+      <c r="E60" s="77"/>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A61" s="44"/>
+      <c r="B61" s="46"/>
+      <c r="C61" s="55"/>
+      <c r="D61" s="56"/>
+      <c r="E61" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6350,18 +7278,18 @@
       <c r="B1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="38"/>
+      <c r="E1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38" t="s">
+      <c r="F1" s="38"/>
+      <c r="G1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -7075,7 +8003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8A15A5-DF59-4294-9A43-F1968F75678E}">
   <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -7093,18 +8021,18 @@
       <c r="B1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="38"/>
+      <c r="E1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38" t="s">
+      <c r="F1" s="38"/>
+      <c r="G1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -7862,18 +8790,18 @@
       <c r="B1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="38"/>
+      <c r="E1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38" t="s">
+      <c r="F1" s="38"/>
+      <c r="G1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>

</xml_diff>